<commit_message>
amount column fixed; added needed doubles for calculation
</commit_message>
<xml_diff>
--- a/res/files/Electric Bills.xlsx
+++ b/res/files/Electric Bills.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -32,13 +32,16 @@
     <t>1</t>
   </si>
   <si>
-    <t>2016-10-16</t>
+    <t>2016-10-15</t>
   </si>
   <si>
-    <t>0909</t>
+    <t>3324</t>
   </si>
   <si>
     <t>LOL AMOUNT</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
@@ -123,6 +126,23 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>